<commit_message>
New data journo folder
</commit_message>
<xml_diff>
--- a/Subjects/ReplacementNames.xlsx
+++ b/Subjects/ReplacementNames.xlsx
@@ -178,8 +178,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="31">
+  <cellStyleXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -218,7 +220,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="31">
+  <cellStyles count="33">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -234,6 +236,7 @@
     <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -249,6 +252,7 @@
     <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -581,7 +585,7 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="A2" sqref="A2:B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -656,7 +660,7 @@
         <v>79</v>
       </c>
       <c r="E4" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:5">

</xml_diff>